<commit_message>
Switched to log-transformed calibration due to vastly improved residuals on low end of calibration. Since the FAME calibration mix is only C24-C32 evens, the means of their slope/intercept are applied to all other FAMEs.
</commit_message>
<xml_diff>
--- a/GC-FID FAMEs Processing Template.xlsx
+++ b/GC-FID FAMEs Processing Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Box Sync\Konecky Lab\Protocols\R Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\KoneckyLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F875C100-16BA-4AD1-8FE8-2AB19E20C2A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA58485-FB3F-49CF-A1E6-1EFB7F60F18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Info" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="57">
   <si>
     <t>comp</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>(ng/µL)</t>
+  </si>
+  <si>
+    <t>batch</t>
   </si>
 </sst>
 </file>
@@ -921,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E392"/>
+  <dimension ref="A1:F392"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -935,7 +938,7 @@
     <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="26" t="s">
         <v>39</v>
       </c>
@@ -951,8 +954,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="20" t="s">
         <v>41</v>
       </c>
@@ -968,8 +974,11 @@
       <c r="E2" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="20" t="s">
         <v>41</v>
       </c>
@@ -985,8 +994,11 @@
       <c r="E3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -1002,8 +1014,11 @@
       <c r="E4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="20" t="s">
         <v>47</v>
       </c>
@@ -1019,8 +1034,11 @@
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="20" t="s">
         <v>47</v>
       </c>
@@ -1036,8 +1054,11 @@
       <c r="E6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
         <v>47</v>
       </c>
@@ -1053,8 +1074,11 @@
       <c r="E7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
         <v>48</v>
       </c>
@@ -1070,8 +1094,11 @@
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="20" t="s">
         <v>48</v>
       </c>
@@ -1087,8 +1114,11 @@
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="20" t="s">
         <v>48</v>
       </c>
@@ -1104,8 +1134,11 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="20" t="s">
         <v>49</v>
       </c>
@@ -1121,8 +1154,11 @@
       <c r="E11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="20" t="s">
         <v>49</v>
       </c>
@@ -1138,8 +1174,11 @@
       <c r="E12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="20" t="s">
         <v>49</v>
       </c>
@@ -1155,8 +1194,11 @@
       <c r="E13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="20" t="s">
         <v>50</v>
       </c>
@@ -1172,8 +1214,11 @@
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="20" t="s">
         <v>50</v>
       </c>
@@ -1189,8 +1234,11 @@
       <c r="E15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="20" t="s">
         <v>50</v>
       </c>
@@ -1206,8 +1254,11 @@
       <c r="E16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="20" t="s">
         <v>51</v>
       </c>
@@ -1223,8 +1274,11 @@
       <c r="E17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="20" t="s">
         <v>51</v>
       </c>
@@ -1240,8 +1294,11 @@
       <c r="E18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="20" t="s">
         <v>51</v>
       </c>
@@ -1257,8 +1314,11 @@
       <c r="E19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
@@ -1274,8 +1334,11 @@
       <c r="E20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="20" t="s">
         <v>52</v>
       </c>
@@ -1291,8 +1354,11 @@
       <c r="E21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="20" t="s">
         <v>52</v>
       </c>
@@ -1308,8 +1374,11 @@
       <c r="E22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="20" t="s">
         <v>53</v>
       </c>
@@ -1325,8 +1394,11 @@
       <c r="E23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="20" t="s">
         <v>53</v>
       </c>
@@ -1342,8 +1414,11 @@
       <c r="E24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="20" t="s">
         <v>53</v>
       </c>
@@ -1359,32 +1434,35 @@
       <c r="E25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="B26"/>
       <c r="C26"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="B27"/>
       <c r="C27"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="B29"/>
       <c r="C29"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="B30"/>
       <c r="C30"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="B31"/>
       <c r="C31"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="B32"/>
       <c r="C32"/>
     </row>
@@ -8355,8 +8433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.8"/>
@@ -8502,10 +8580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -8516,7 +8594,7 @@
     <col min="4" max="16384" width="9.109375" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
@@ -8526,8 +8604,11 @@
       <c r="C1" s="22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="21">
         <v>0</v>
       </c>
@@ -8537,8 +8618,11 @@
       <c r="C2" s="21">
         <v>1919.8679999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="21">
         <v>0</v>
       </c>
@@ -8548,8 +8632,11 @@
       <c r="C3" s="21">
         <v>1903.261</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="21">
         <v>0</v>
       </c>
@@ -8559,8 +8646,11 @@
       <c r="C4" s="21">
         <v>1950.76</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="21">
         <v>0</v>
       </c>
@@ -8570,8 +8660,11 @@
       <c r="C5" s="21">
         <v>1967.511</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="21">
         <v>0</v>
       </c>
@@ -8581,8 +8674,11 @@
       <c r="C6" s="21">
         <v>1930.0329999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="21">
         <v>1</v>
       </c>
@@ -8592,8 +8688,11 @@
       <c r="C7" s="21">
         <v>952.33399999999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="21">
         <v>1</v>
       </c>
@@ -8603,8 +8702,11 @@
       <c r="C8" s="21">
         <v>943.56500000000005</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -8614,8 +8716,11 @@
       <c r="C9" s="21">
         <v>966.44899999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="21">
         <v>1</v>
       </c>
@@ -8625,8 +8730,11 @@
       <c r="C10" s="21">
         <v>973.26499999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="21">
         <v>1</v>
       </c>
@@ -8636,8 +8744,11 @@
       <c r="C11" s="21">
         <v>962.66099999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="21">
         <v>2</v>
       </c>
@@ -8647,8 +8758,11 @@
       <c r="C12" s="21">
         <v>529.48699999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="21">
         <v>2</v>
       </c>
@@ -8658,8 +8772,11 @@
       <c r="C13" s="21">
         <v>532.04700000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="21">
         <v>2</v>
       </c>
@@ -8669,8 +8786,11 @@
       <c r="C14" s="21">
         <v>524.59</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="21">
         <v>2</v>
       </c>
@@ -8680,8 +8800,11 @@
       <c r="C15" s="21">
         <v>521.69399999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="21">
         <v>2</v>
       </c>
@@ -8691,8 +8814,11 @@
       <c r="C16" s="21">
         <v>496.16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="21">
         <v>2</v>
       </c>
@@ -8702,8 +8828,11 @@
       <c r="C17" s="21">
         <v>521.70500000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="21">
         <v>2</v>
       </c>
@@ -8713,8 +8842,11 @@
       <c r="C18" s="21">
         <v>525.31100000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="21">
         <v>2</v>
       </c>
@@ -8724,8 +8856,11 @@
       <c r="C19" s="21">
         <v>518.43600000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="21">
         <v>2</v>
       </c>
@@ -8735,8 +8870,11 @@
       <c r="C20" s="21">
         <v>491.47300000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="21">
         <v>2</v>
       </c>
@@ -8746,8 +8884,11 @@
       <c r="C21" s="21">
         <v>515.98599999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="21">
         <v>2</v>
       </c>
@@ -8757,8 +8898,11 @@
       <c r="C22" s="21">
         <v>529.80499999999995</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="21">
         <v>2</v>
       </c>
@@ -8768,8 +8912,11 @@
       <c r="C23" s="21">
         <v>533.024</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="21">
         <v>2</v>
       </c>
@@ -8779,8 +8926,11 @@
       <c r="C24" s="21">
         <v>536.24800000000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="21">
         <v>2</v>
       </c>
@@ -8790,8 +8940,11 @@
       <c r="C25" s="21">
         <v>527.25099999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="21">
         <v>2</v>
       </c>
@@ -8801,8 +8954,11 @@
       <c r="C26" s="21">
         <v>502.48500000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="21">
         <v>2</v>
       </c>
@@ -8812,8 +8968,11 @@
       <c r="C27" s="21">
         <v>537.00400000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="21">
         <v>2</v>
       </c>
@@ -8823,8 +8982,11 @@
       <c r="C28" s="21">
         <v>531.82799999999997</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="21">
         <v>2</v>
       </c>
@@ -8834,8 +8996,11 @@
       <c r="C29" s="21">
         <v>533.69500000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="21">
         <v>2</v>
       </c>
@@ -8845,8 +9010,11 @@
       <c r="C30" s="21">
         <v>539.41600000000005</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="21">
         <v>2</v>
       </c>
@@ -8856,8 +9024,11 @@
       <c r="C31" s="21">
         <v>505.42500000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="21">
         <v>2</v>
       </c>
@@ -8867,8 +9038,11 @@
       <c r="C32" s="21">
         <v>487.83499999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="21">
         <v>2</v>
       </c>
@@ -8878,8 +9052,11 @@
       <c r="C33" s="21">
         <v>524.50300000000004</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="21">
         <v>2</v>
       </c>
@@ -8889,8 +9066,11 @@
       <c r="C34" s="21">
         <v>525.67700000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="21">
         <v>2</v>
       </c>
@@ -8900,8 +9080,11 @@
       <c r="C35" s="21">
         <v>528.81399999999996</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="21">
         <v>2</v>
       </c>
@@ -8911,8 +9094,11 @@
       <c r="C36" s="21">
         <v>520.70299999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="21">
         <v>3</v>
       </c>
@@ -8922,8 +9108,11 @@
       <c r="C37" s="21">
         <v>252.83699999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="21">
         <v>3</v>
       </c>
@@ -8933,8 +9122,11 @@
       <c r="C38" s="21">
         <v>250.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="21">
         <v>3</v>
       </c>
@@ -8944,8 +9136,11 @@
       <c r="C39" s="21">
         <v>255.36</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="21">
         <v>3</v>
       </c>
@@ -8955,8 +9150,11 @@
       <c r="C40" s="21">
         <v>256.64699999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="21">
         <v>3</v>
       </c>
@@ -8966,8 +9164,11 @@
       <c r="C41" s="21">
         <v>246.98699999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="21">
         <v>4</v>
       </c>
@@ -8977,8 +9178,11 @@
       <c r="C42" s="21">
         <v>124.658</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="21">
         <v>4</v>
       </c>
@@ -8988,8 +9192,11 @@
       <c r="C43" s="21">
         <v>123.51</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="21">
         <v>4</v>
       </c>
@@ -8999,8 +9206,11 @@
       <c r="C44" s="21">
         <v>125.648</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="21">
         <v>4</v>
       </c>
@@ -9010,8 +9220,11 @@
       <c r="C45" s="21">
         <v>126.095</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="21">
         <v>4</v>
       </c>
@@ -9021,13 +9234,16 @@
       <c r="C46" s="21">
         <v>122.202</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="24"/>
       <c r="B47" s="22"/>
       <c r="C47" s="24"/>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48" s="24"/>
       <c r="B48" s="22"/>
       <c r="C48" s="24"/>

</xml_diff>